<commit_message>
Today, 29 Oct, I concluded Enn payments and optimized errorlog...
</commit_message>
<xml_diff>
--- a/ALL DATA TO SQLITE STATIC AND JOURNAL.xlsx
+++ b/ALL DATA TO SQLITE STATIC AND JOURNAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 WORK 2017\2 general\00 2018 TEVIN\OUR ETR\CharmSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tevin\CoreOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67F5E04A-64CC-4242-87B5-663567EA4739}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9705A30E-B1C4-4EAA-AC2C-176008D6AB05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26610" windowHeight="9495" activeTab="6" xr2:uid="{EE25166E-B9FA-48BB-BDE6-89282C202F97}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26616" windowHeight="9492" activeTab="10" xr2:uid="{EE25166E-B9FA-48BB-BDE6-89282C202F97}"/>
   </bookViews>
   <sheets>
     <sheet name="PLU" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,24 @@
     <sheet name="ejournal" sheetId="7" r:id="rId8"/>
     <sheet name="details" sheetId="8" r:id="rId9"/>
     <sheet name="state" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="336">
   <si>
     <t>barcode</t>
   </si>
@@ -1090,6 +1096,21 @@
   </si>
   <si>
     <t xml:space="preserve">null </t>
+  </si>
+  <si>
+    <t>apoforologisi</t>
+  </si>
+  <si>
+    <t>gross</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>vatrate</t>
   </si>
 </sst>
 </file>
@@ -1495,14 +1516,14 @@
       <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="22" max="22" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>8801</v>
       </c>
@@ -1636,7 +1657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>8802</v>
       </c>
@@ -1704,7 +1725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>8803</v>
       </c>
@@ -1772,7 +1793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>8804</v>
       </c>
@@ -1840,7 +1861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>8805</v>
       </c>
@@ -1908,7 +1929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>8806</v>
       </c>
@@ -1976,7 +1997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>8807</v>
       </c>
@@ -2044,7 +2065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8808</v>
       </c>
@@ -2112,7 +2133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8809</v>
       </c>
@@ -2180,7 +2201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8810</v>
       </c>
@@ -2248,7 +2269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>8811</v>
       </c>
@@ -2316,7 +2337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>90</v>
       </c>
@@ -2384,7 +2405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>91</v>
       </c>
@@ -2452,7 +2473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>92</v>
       </c>
@@ -2520,7 +2541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>93</v>
       </c>
@@ -2588,7 +2609,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>94</v>
       </c>
@@ -2656,7 +2677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2724,7 +2745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2779,17 +2800,17 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>274</v>
       </c>
@@ -2819,6 +2840,60 @@
       </c>
       <c r="J1" s="4" t="s">
         <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2209DFD6-C095-4CAA-9B0F-F228E7D9C971}">
+  <dimension ref="D3:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>334</v>
+      </c>
+      <c r="I5">
+        <f>E5/(1+(E6/100))</f>
+        <v>108.8495575221239</v>
+      </c>
+      <c r="K5">
+        <f>I5+I5*(0.13)</f>
+        <v>123.00000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>333</v>
+      </c>
+      <c r="I6">
+        <f>E5-I5</f>
+        <v>14.150442477876098</v>
       </c>
     </row>
   </sheetData>
@@ -2837,12 +2912,12 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -2886,7 +2961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -2930,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -2974,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -3018,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
@@ -3062,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -3106,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
@@ -3150,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
@@ -3194,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -3238,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3282,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
@@ -3326,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -3370,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
@@ -3414,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -3458,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -3502,7 +3577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -3562,14 +3637,14 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>99</v>
       </c>
@@ -3583,7 +3658,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3597,7 +3672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3611,7 +3686,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3625,7 +3700,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3639,7 +3714,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3669,9 +3744,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -3697,7 +3772,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6.5</v>
       </c>
@@ -3739,25 +3814,25 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -3822,7 +3897,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3894,18 +3969,18 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="4"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>204</v>
       </c>
@@ -3934,7 +4009,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -3951,7 +4026,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -3968,7 +4043,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3985,7 +4060,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -4002,7 +4077,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -4019,7 +4094,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -4036,7 +4111,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -4053,7 +4128,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -4070,7 +4145,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>218</v>
       </c>
@@ -4087,7 +4162,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>218</v>
       </c>
@@ -4104,7 +4179,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>218</v>
       </c>
@@ -4121,7 +4196,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>222</v>
       </c>
@@ -4138,7 +4213,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>222</v>
       </c>
@@ -4155,7 +4230,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>222</v>
       </c>
@@ -4172,7 +4247,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>242</v>
       </c>
@@ -4189,7 +4264,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -4206,7 +4281,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4223,7 +4298,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>236</v>
       </c>
@@ -4240,7 +4315,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>236</v>
       </c>
@@ -4257,7 +4332,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>236</v>
       </c>
@@ -4287,39 +4362,39 @@
   </sheetPr>
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" customWidth="1"/>
-    <col min="16" max="17" width="22.140625" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" customWidth="1"/>
+    <col min="16" max="17" width="22.109375" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" customWidth="1"/>
     <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="22" width="17.7109375" customWidth="1"/>
+    <col min="21" max="22" width="17.6640625" customWidth="1"/>
     <col min="23" max="24" width="15" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" customWidth="1"/>
-    <col min="26" max="26" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" customWidth="1"/>
+    <col min="26" max="26" width="15.88671875" customWidth="1"/>
     <col min="27" max="27" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>288</v>
       </c>
@@ -4402,7 +4477,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4485,7 +4560,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4499,7 +4574,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4520,17 +4595,17 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="5"/>
+    <col min="1" max="3" width="9.109375" style="5"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="5"/>
-    <col min="8" max="9" width="15.5703125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="5" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="5"/>
+    <col min="8" max="9" width="15.5546875" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>154</v>
       </c>
@@ -4616,7 +4691,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4696,7 +4771,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4776,7 +4851,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -4856,7 +4931,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -4936,7 +5011,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -5016,7 +5091,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -5096,7 +5171,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -5176,7 +5251,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -5256,7 +5331,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -5336,7 +5411,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -5416,7 +5491,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -5496,7 +5571,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -5576,7 +5651,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -5656,7 +5731,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -5736,7 +5811,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>1</v>
       </c>
@@ -5816,7 +5891,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>1</v>
       </c>
@@ -5896,7 +5971,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -5976,7 +6051,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -6056,7 +6131,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -6152,27 +6227,27 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="18" width="10.5703125" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="11" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" customWidth="1"/>
+    <col min="17" max="18" width="10.5546875" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>154</v>
       </c>
@@ -6255,7 +6330,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>